<commit_message>
Rewrote the isAdjacent function We now pass all of our own tests and Prof. Rader's tests
</commit_message>
<xml_diff>
--- a/Gameboard Outline.xlsx
+++ b/Gameboard Outline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3420" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3072,8 +3072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N42" sqref="C32:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3164,103 +3164,103 @@
         <v>0</v>
       </c>
       <c r="B2" s="18">
-        <f>$A2 *25 + B$1</f>
+        <f t="shared" ref="B2:K11" si="0">$A2 *25 + B$1</f>
         <v>0</v>
       </c>
       <c r="C2" s="12">
-        <f>$A2 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D2" s="12">
-        <f>$A2 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E2" s="12">
-        <f>$A2 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F2" s="2">
-        <f>$A2 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G2" s="25">
-        <f>$A2 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H2" s="2">
-        <f>$A2 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I2" s="12">
-        <f>$A2 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J2" s="12">
-        <f>$A2 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K2" s="12">
-        <f>$A2 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L2" s="12">
-        <f>$A2 *25 + L$1</f>
+        <f t="shared" ref="L2:Z11" si="1">$A2 *25 + L$1</f>
         <v>10</v>
       </c>
       <c r="M2" s="2">
-        <f>$A2 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="N2" s="2">
-        <f>$A2 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="O2" s="12">
-        <f>$A2 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="P2" s="12">
-        <f>$A2 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="Q2" s="12">
-        <f>$A2 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="R2" s="12">
-        <f>$A2 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="S2" s="12">
-        <f>$A2 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="T2" s="2">
-        <f>$A2 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="U2" s="2">
-        <f>$A2 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="V2" s="2">
-        <f>$A2 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="W2" s="12">
-        <f>$A2 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="X2" s="12">
-        <f>$A2 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="Y2" s="12">
-        <f>$A2 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="Z2" s="13">
-        <f>$A2 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -3269,103 +3269,103 @@
         <v>1</v>
       </c>
       <c r="B3" s="14">
-        <f>$A3 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C3" s="8">
-        <f>$A3 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="D3" s="8">
-        <f>$A3 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E3" s="8">
-        <f>$A3 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="F3" s="8">
-        <f>$A3 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="G3" s="3">
-        <f>$A3 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="H3" s="3">
-        <f>$A3 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="I3" s="8">
-        <f>$A3 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="J3" s="8">
-        <f>$A3 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="K3" s="8">
-        <f>$A3 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="L3" s="8">
-        <f>$A3 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="M3" s="8">
-        <f>$A3 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="N3" s="3">
-        <f>$A3 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="O3" s="8">
-        <f>$A3 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="P3" s="8">
-        <f>$A3 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="Q3" s="8">
-        <f>$A3 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="R3" s="8">
-        <f>$A3 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="S3" s="8">
-        <f>$A3 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="T3" s="3">
-        <f>$A3 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="U3" s="3">
-        <f>$A3 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="V3" s="3">
-        <f>$A3 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="W3" s="8">
-        <f>$A3 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="X3" s="8">
-        <f>$A3 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="Y3" s="8">
-        <f>$A3 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="Z3" s="10">
-        <f>$A3 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
     </row>
@@ -3374,103 +3374,103 @@
         <v>2</v>
       </c>
       <c r="B4" s="14">
-        <f>$A4 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="C4" s="8">
-        <f>$A4 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="D4" s="8">
-        <f>$A4 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E4" s="8">
-        <f>$A4 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="F4" s="8">
-        <f>$A4 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="G4" s="3">
-        <f>$A4 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="H4" s="3">
-        <f>$A4 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="I4" s="8">
-        <f>$A4 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="J4" s="8">
-        <f>$A4 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="K4" s="8">
-        <f>$A4 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="L4" s="8">
-        <f>$A4 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="M4" s="8">
-        <f>$A4 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="N4" s="3">
-        <f>$A4 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="O4" s="37">
-        <f>$A4 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="P4" s="8">
-        <f>$A4 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="Q4" s="8">
-        <f>$A4 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="R4" s="8">
-        <f>$A4 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="S4" s="8">
-        <f>$A4 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="T4" s="3">
-        <f>$A4 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="U4" s="3">
-        <f>$A4 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="V4" s="8">
-        <f>$A4 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="W4" s="8">
-        <f>$A4 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="X4" s="8">
-        <f>$A4 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="Y4" s="8">
-        <f>$A4 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="Z4" s="10">
-        <f>$A4 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
@@ -3479,103 +3479,103 @@
         <v>3</v>
       </c>
       <c r="B5" s="14">
-        <f>$A5 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="C5" s="8">
-        <f>$A5 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="D5" s="8">
-        <f>$A5 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="E5" s="8">
-        <f>$A5 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="F5" s="8">
-        <f>$A5 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="G5" s="3">
-        <f>$A5 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="H5" s="3">
-        <f>$A5 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="I5" s="8">
-        <f>$A5 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="J5" s="8">
-        <f>$A5 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="K5" s="8">
-        <f>$A5 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="L5" s="8">
-        <f>$A5 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="M5" s="8">
-        <f>$A5 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="N5" s="36">
-        <f>$A5 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="O5" s="8">
-        <f>$A5 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="P5" s="8">
-        <f>$A5 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="Q5" s="8">
-        <f>$A5 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="R5" s="8">
-        <f>$A5 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="S5" s="8">
-        <f>$A5 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="T5" s="3">
-        <f>$A5 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="U5" s="3">
-        <f>$A5 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="V5" s="8">
-        <f>$A5 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="W5" s="8">
-        <f>$A5 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="X5" s="8">
-        <f>$A5 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="Y5" s="8">
-        <f>$A5 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="Z5" s="10">
-        <f>$A5 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
@@ -3584,103 +3584,103 @@
         <v>4</v>
       </c>
       <c r="B6" s="14">
-        <f>$A6 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C6" s="8">
-        <f>$A6 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="D6" s="8">
-        <f>$A6 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="E6" s="8">
-        <f>$A6 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="F6" s="8">
-        <f>$A6 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="G6" s="3">
-        <f>$A6 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="H6" s="3">
-        <f>$A6 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="I6" s="8">
-        <f>$A6 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="J6" s="8">
-        <f>$A6 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="K6" s="8">
-        <f>$A6 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="L6" s="8">
-        <f>$A6 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="M6" s="8">
-        <f>$A6 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="N6" s="3">
-        <f>$A6 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="O6" s="8">
-        <f>$A6 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>113</v>
       </c>
       <c r="P6" s="8">
-        <f>$A6 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>114</v>
       </c>
       <c r="Q6" s="8">
-        <f>$A6 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="R6" s="8">
-        <f>$A6 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="S6" s="8">
-        <f>$A6 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="T6" s="3">
-        <f>$A6 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="U6" s="3">
-        <f>$A6 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="V6" s="8">
-        <f>$A6 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="W6" s="8">
-        <f>$A6 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>121</v>
       </c>
       <c r="X6" s="8">
-        <f>$A6 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>122</v>
       </c>
       <c r="Y6" s="8">
-        <f>$A6 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="Z6" s="10">
-        <f>$A6 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
     </row>
@@ -3689,103 +3689,103 @@
         <v>5</v>
       </c>
       <c r="B7" s="14">
-        <f>$A7 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="C7" s="8">
-        <f>$A7 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="D7" s="8">
-        <f>$A7 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="E7" s="8">
-        <f>$A7 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="F7" s="8">
-        <f>$A7 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="G7" s="3">
-        <f>$A7 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="H7" s="3">
-        <f>$A7 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="I7" s="8">
-        <f>$A7 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="J7" s="8">
-        <f>$A7 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="K7" s="8">
-        <f>$A7 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>134</v>
       </c>
       <c r="L7" s="8">
-        <f>$A7 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="M7" s="7">
-        <f>$A7 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="N7" s="3">
-        <f>$A7 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>137</v>
       </c>
       <c r="O7" s="8">
-        <f>$A7 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="P7" s="8">
-        <f>$A7 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
       <c r="Q7" s="8">
-        <f>$A7 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="R7" s="8">
-        <f>$A7 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>141</v>
       </c>
       <c r="S7" s="8">
-        <f>$A7 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="T7" s="3">
-        <f>$A7 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>143</v>
       </c>
       <c r="U7" s="3">
-        <f>$A7 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
       <c r="V7" s="7">
-        <f>$A7 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
       <c r="W7" s="8">
-        <f>$A7 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="X7" s="8">
-        <f>$A7 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
       <c r="Y7" s="8">
-        <f>$A7 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>148</v>
       </c>
       <c r="Z7" s="10">
-        <f>$A7 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>149</v>
       </c>
     </row>
@@ -3794,103 +3794,103 @@
         <v>6</v>
       </c>
       <c r="B8" s="14">
-        <f>$A8 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="C8" s="8">
-        <f>$A8 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>151</v>
       </c>
       <c r="D8" s="8">
-        <f>$A8 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="E8" s="32">
-        <f>$A8 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>153</v>
       </c>
       <c r="F8" s="3">
-        <f>$A8 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="G8" s="3">
-        <f>$A8 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="H8" s="3">
-        <f>$A8 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="I8" s="8">
-        <f>$A8 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="J8" s="7">
-        <f>$A8 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="K8" s="8">
-        <f>$A8 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>159</v>
       </c>
       <c r="L8" s="8">
-        <f>$A8 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="M8" s="8">
-        <f>$A8 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>161</v>
       </c>
       <c r="N8" s="3">
-        <f>$A8 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="O8" s="3">
-        <f>$A8 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>163</v>
       </c>
       <c r="P8" s="8">
-        <f>$A8 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>164</v>
       </c>
       <c r="Q8" s="7">
-        <f>$A8 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
       <c r="R8" s="8">
-        <f>$A8 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>166</v>
       </c>
       <c r="S8" s="3">
-        <f>$A8 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>167</v>
       </c>
       <c r="T8" s="3">
-        <f>$A8 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="U8" s="3">
-        <f>$A8 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="V8" s="3">
-        <f>$A8 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>170</v>
       </c>
       <c r="W8" s="8">
-        <f>$A8 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>171</v>
       </c>
       <c r="X8" s="8">
-        <f>$A8 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>172</v>
       </c>
       <c r="Y8" s="8">
-        <f>$A8 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>173</v>
       </c>
       <c r="Z8" s="6">
-        <f>$A8 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>174</v>
       </c>
     </row>
@@ -3899,103 +3899,103 @@
         <v>7</v>
       </c>
       <c r="B9" s="5">
-        <f>$A9 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="C9" s="3">
-        <f>$A9 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="D9" s="3">
-        <f>$A9 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>177</v>
       </c>
       <c r="E9" s="3">
-        <f>$A9 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="F9" s="3">
-        <f>$A9 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>179</v>
       </c>
       <c r="G9" s="3">
-        <f>$A9 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="H9" s="3">
-        <f>$A9 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>181</v>
       </c>
       <c r="I9" s="3">
-        <f>$A9 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>182</v>
       </c>
       <c r="J9" s="30">
-        <f>$A9 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>183</v>
       </c>
       <c r="K9" s="3">
-        <f>$A9 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>184</v>
       </c>
       <c r="L9" s="3">
-        <f>$A9 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="M9" s="3">
-        <f>$A9 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="N9" s="3">
-        <f>$A9 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
       <c r="O9" s="3">
-        <f>$A9 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>188</v>
       </c>
       <c r="P9" s="3">
-        <f>$A9 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>189</v>
       </c>
       <c r="Q9" s="3">
-        <f>$A9 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
       <c r="R9" s="3">
-        <f>$A9 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>191</v>
       </c>
       <c r="S9" s="3">
-        <f>$A9 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>192</v>
       </c>
       <c r="T9" s="35">
-        <f>$A9 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>193</v>
       </c>
       <c r="U9" s="3">
-        <f>$A9 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="V9" s="3">
-        <f>$A9 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
       <c r="W9" s="3">
-        <f>$A9 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>196</v>
       </c>
       <c r="X9" s="3">
-        <f>$A9 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>197</v>
       </c>
       <c r="Y9" s="3">
-        <f>$A9 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>198</v>
       </c>
       <c r="Z9" s="26">
-        <f>$A9 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>199</v>
       </c>
     </row>
@@ -4004,103 +4004,103 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <f>$A10 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="C10" s="3">
-        <f>$A10 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>201</v>
       </c>
       <c r="D10" s="3">
-        <f>$A10 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>202</v>
       </c>
       <c r="E10" s="3">
-        <f>$A10 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>203</v>
       </c>
       <c r="F10" s="3">
-        <f>$A10 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>204</v>
       </c>
       <c r="G10" s="3">
-        <f>$A10 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
       <c r="H10" s="35">
-        <f>$A10 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>206</v>
       </c>
       <c r="I10" s="3">
-        <f>$A10 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>207</v>
       </c>
       <c r="J10" s="3">
-        <f>$A10 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="K10" s="3">
-        <f>$A10 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="L10" s="3">
-        <f>$A10 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="M10" s="3">
-        <f>$A10 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>211</v>
       </c>
       <c r="N10" s="3">
-        <f>$A10 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>212</v>
       </c>
       <c r="O10" s="3">
-        <f>$A10 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>213</v>
       </c>
       <c r="P10" s="3">
-        <f>$A10 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>214</v>
       </c>
       <c r="Q10" s="3">
-        <f>$A10 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
       <c r="R10" s="3">
-        <f>$A10 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
       <c r="S10" s="3">
-        <f>$A10 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>217</v>
       </c>
       <c r="T10" s="3">
-        <f>$A10 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>218</v>
       </c>
       <c r="U10" s="3">
-        <f>$A10 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>219</v>
       </c>
       <c r="V10" s="3">
-        <f>$A10 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="W10" s="3">
-        <f>$A10 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>221</v>
       </c>
       <c r="X10" s="3">
-        <f>$A10 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>222</v>
       </c>
       <c r="Y10" s="3">
-        <f>$A10 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>223</v>
       </c>
       <c r="Z10" s="6">
-        <f>$A10 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>224</v>
       </c>
     </row>
@@ -4109,103 +4109,103 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <f>$A11 *25 + B$1</f>
+        <f t="shared" si="0"/>
         <v>225</v>
       </c>
       <c r="C11" s="3">
-        <f>$A11 *25 + C$1</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="D11" s="3">
-        <f>$A11 *25 + D$1</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="E11" s="28">
-        <f>$A11 *25 + E$1</f>
+        <f t="shared" si="0"/>
         <v>228</v>
       </c>
       <c r="F11" s="3">
-        <f>$A11 *25 + F$1</f>
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
       <c r="G11" s="3">
-        <f>$A11 *25 + G$1</f>
+        <f t="shared" si="0"/>
         <v>230</v>
       </c>
       <c r="H11" s="3">
-        <f>$A11 *25 + H$1</f>
+        <f t="shared" si="0"/>
         <v>231</v>
       </c>
       <c r="I11" s="3">
-        <f>$A11 *25 + I$1</f>
+        <f t="shared" si="0"/>
         <v>232</v>
       </c>
       <c r="J11" s="3">
-        <f>$A11 *25 + J$1</f>
+        <f t="shared" si="0"/>
         <v>233</v>
       </c>
       <c r="K11" s="1">
-        <f>$A11 *25 + K$1</f>
+        <f t="shared" si="0"/>
         <v>234</v>
       </c>
       <c r="L11" s="1">
-        <f>$A11 *25 + L$1</f>
+        <f t="shared" si="1"/>
         <v>235</v>
       </c>
       <c r="M11" s="1">
-        <f>$A11 *25 + M$1</f>
+        <f t="shared" si="1"/>
         <v>236</v>
       </c>
       <c r="N11" s="1">
-        <f>$A11 *25 + N$1</f>
+        <f t="shared" si="1"/>
         <v>237</v>
       </c>
       <c r="O11" s="1">
-        <f>$A11 *25 + O$1</f>
+        <f t="shared" si="1"/>
         <v>238</v>
       </c>
       <c r="P11" s="1">
-        <f>$A11 *25 + P$1</f>
+        <f t="shared" si="1"/>
         <v>239</v>
       </c>
       <c r="Q11" s="1">
-        <f>$A11 *25 + Q$1</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="R11" s="3">
-        <f>$A11 *25 + R$1</f>
+        <f t="shared" si="1"/>
         <v>241</v>
       </c>
       <c r="S11" s="3">
-        <f>$A11 *25 + S$1</f>
+        <f t="shared" si="1"/>
         <v>242</v>
       </c>
       <c r="T11" s="3">
-        <f>$A11 *25 + T$1</f>
+        <f t="shared" si="1"/>
         <v>243</v>
       </c>
       <c r="U11" s="8">
-        <f>$A11 *25 + U$1</f>
+        <f t="shared" si="1"/>
         <v>244</v>
       </c>
       <c r="V11" s="8">
-        <f>$A11 *25 + V$1</f>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
       <c r="W11" s="8">
-        <f>$A11 *25 + W$1</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="X11" s="8">
-        <f>$A11 *25 + X$1</f>
+        <f t="shared" si="1"/>
         <v>247</v>
       </c>
       <c r="Y11" s="8">
-        <f>$A11 *25 + Y$1</f>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
       <c r="Z11" s="10">
-        <f>$A11 *25 + Z$1</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
     </row>
@@ -4214,103 +4214,103 @@
         <v>10</v>
       </c>
       <c r="B12" s="14">
-        <f>$A12 *25 + B$1</f>
+        <f t="shared" ref="B12:K26" si="2">$A12 *25 + B$1</f>
         <v>250</v>
       </c>
       <c r="C12" s="8">
-        <f>$A12 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>251</v>
       </c>
       <c r="D12" s="8">
-        <f>$A12 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
       <c r="E12" s="8">
-        <f>$A12 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>253</v>
       </c>
       <c r="F12" s="8">
-        <f>$A12 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>254</v>
       </c>
       <c r="G12" s="8">
-        <f>$A12 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="H12" s="3">
-        <f>$A12 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="I12" s="3">
-        <f>$A12 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>257</v>
       </c>
       <c r="J12" s="3">
-        <f>$A12 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>258</v>
       </c>
       <c r="K12" s="1">
-        <f>$A12 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>259</v>
       </c>
       <c r="L12" s="1">
-        <f>$A12 *25 + L$1</f>
+        <f t="shared" ref="L12:Z26" si="3">$A12 *25 + L$1</f>
         <v>260</v>
       </c>
       <c r="M12" s="1">
-        <f>$A12 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="N12" s="1">
-        <f>$A12 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>262</v>
       </c>
       <c r="O12" s="1">
-        <f>$A12 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>263</v>
       </c>
       <c r="P12" s="1">
-        <f>$A12 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>264</v>
       </c>
       <c r="Q12" s="1">
-        <f>$A12 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>265</v>
       </c>
       <c r="R12" s="3">
-        <f>$A12 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>266</v>
       </c>
       <c r="S12" s="3">
-        <f>$A12 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>267</v>
       </c>
       <c r="T12" s="3">
-        <f>$A12 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>268</v>
       </c>
       <c r="U12" s="8">
-        <f>$A12 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>269</v>
       </c>
       <c r="V12" s="8">
-        <f>$A12 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="W12" s="8">
-        <f>$A12 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>271</v>
       </c>
       <c r="X12" s="8">
-        <f>$A12 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="Y12" s="8">
-        <f>$A12 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>273</v>
       </c>
       <c r="Z12" s="10">
-        <f>$A12 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>274</v>
       </c>
     </row>
@@ -4319,103 +4319,103 @@
         <v>11</v>
       </c>
       <c r="B13" s="14">
-        <f>$A13 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>275</v>
       </c>
       <c r="C13" s="8">
-        <f>$A13 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>276</v>
       </c>
       <c r="D13" s="8">
-        <f>$A13 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>277</v>
       </c>
       <c r="E13" s="8">
-        <f>$A13 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>278</v>
       </c>
       <c r="F13" s="8">
-        <f>$A13 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>279</v>
       </c>
       <c r="G13" s="8">
-        <f>$A13 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>280</v>
       </c>
       <c r="H13" s="3">
-        <f>$A13 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>281</v>
       </c>
       <c r="I13" s="3">
-        <f>$A13 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>282</v>
       </c>
       <c r="J13" s="3">
-        <f>$A13 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>283</v>
       </c>
       <c r="K13" s="1">
-        <f>$A13 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>284</v>
       </c>
       <c r="L13" s="1">
-        <f>$A13 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>285</v>
       </c>
       <c r="M13" s="1">
-        <f>$A13 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>286</v>
       </c>
       <c r="N13" s="1">
-        <f>$A13 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>287</v>
       </c>
       <c r="O13" s="1">
-        <f>$A13 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>288</v>
       </c>
       <c r="P13" s="1">
-        <f>$A13 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="Q13" s="1">
-        <f>$A13 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>290</v>
       </c>
       <c r="R13" s="3">
-        <f>$A13 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>291</v>
       </c>
       <c r="S13" s="3">
-        <f>$A13 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>292</v>
       </c>
       <c r="T13" s="3">
-        <f>$A13 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>293</v>
       </c>
       <c r="U13" s="7">
-        <f>$A13 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>294</v>
       </c>
       <c r="V13" s="8">
-        <f>$A13 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>295</v>
       </c>
       <c r="W13" s="8">
-        <f>$A13 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>296</v>
       </c>
       <c r="X13" s="8">
-        <f>$A13 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>297</v>
       </c>
       <c r="Y13" s="8">
-        <f>$A13 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="Z13" s="10">
-        <f>$A13 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>299</v>
       </c>
     </row>
@@ -4424,103 +4424,103 @@
         <v>12</v>
       </c>
       <c r="B14" s="14">
-        <f>$A14 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="C14" s="8">
-        <f>$A14 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>301</v>
       </c>
       <c r="D14" s="8">
-        <f>$A14 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>302</v>
       </c>
       <c r="E14" s="8">
-        <f>$A14 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>303</v>
       </c>
       <c r="F14" s="8">
-        <f>$A14 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>304</v>
       </c>
       <c r="G14" s="7">
-        <f>$A14 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>305</v>
       </c>
       <c r="H14" s="3">
-        <f>$A14 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>306</v>
       </c>
       <c r="I14" s="3">
-        <f>$A14 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>307</v>
       </c>
       <c r="J14" s="3">
-        <f>$A14 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>308</v>
       </c>
       <c r="K14" s="1">
-        <f>$A14 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>309</v>
       </c>
       <c r="L14" s="1">
-        <f>$A14 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>310</v>
       </c>
       <c r="M14" s="1">
-        <f>$A14 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>311</v>
       </c>
       <c r="N14" s="1">
-        <f>$A14 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>312</v>
       </c>
       <c r="O14" s="1">
-        <f>$A14 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>313</v>
       </c>
       <c r="P14" s="1">
-        <f>$A14 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>314</v>
       </c>
       <c r="Q14" s="1">
-        <f>$A14 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
       <c r="R14" s="3">
-        <f>$A14 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>316</v>
       </c>
       <c r="S14" s="3">
-        <f>$A14 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>317</v>
       </c>
       <c r="T14" s="30">
-        <f>$A14 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>318</v>
       </c>
       <c r="U14" s="7">
-        <f>$A14 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>319</v>
       </c>
       <c r="V14" s="8">
-        <f>$A14 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>320</v>
       </c>
       <c r="W14" s="8">
-        <f>$A14 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>321</v>
       </c>
       <c r="X14" s="8">
-        <f>$A14 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>322</v>
       </c>
       <c r="Y14" s="8">
-        <f>$A14 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="Z14" s="10">
-        <f>$A14 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>324</v>
       </c>
     </row>
@@ -4529,103 +4529,103 @@
         <v>13</v>
       </c>
       <c r="B15" s="14">
-        <f>$A15 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>325</v>
       </c>
       <c r="C15" s="8">
-        <f>$A15 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>326</v>
       </c>
       <c r="D15" s="8">
-        <f>$A15 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>327</v>
       </c>
       <c r="E15" s="8">
-        <f>$A15 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>328</v>
       </c>
       <c r="F15" s="8">
-        <f>$A15 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>329</v>
       </c>
       <c r="G15" s="7">
-        <f>$A15 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>330</v>
       </c>
       <c r="H15" s="3">
-        <f>$A15 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>331</v>
       </c>
       <c r="I15" s="3">
-        <f>$A15 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>332</v>
       </c>
       <c r="J15" s="3">
-        <f>$A15 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>333</v>
       </c>
       <c r="K15" s="1">
-        <f>$A15 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>334</v>
       </c>
       <c r="L15" s="1">
-        <f>$A15 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>335</v>
       </c>
       <c r="M15" s="1">
-        <f>$A15 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>336</v>
       </c>
       <c r="N15" s="1">
-        <f>$A15 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>337</v>
       </c>
       <c r="O15" s="1">
-        <f>$A15 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>338</v>
       </c>
       <c r="P15" s="1">
-        <f>$A15 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>339</v>
       </c>
       <c r="Q15" s="1">
-        <f>$A15 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>340</v>
       </c>
       <c r="R15" s="3">
-        <f>$A15 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>341</v>
       </c>
       <c r="S15" s="35">
-        <f>$A15 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>342</v>
       </c>
       <c r="T15" s="3">
-        <f>$A15 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>343</v>
       </c>
       <c r="U15" s="8">
-        <f>$A15 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>344</v>
       </c>
       <c r="V15" s="8">
-        <f>$A15 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>345</v>
       </c>
       <c r="W15" s="8">
-        <f>$A15 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>346</v>
       </c>
       <c r="X15" s="8">
-        <f>$A15 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>347</v>
       </c>
       <c r="Y15" s="8">
-        <f>$A15 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>348</v>
       </c>
       <c r="Z15" s="10">
-        <f>$A15 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>349</v>
       </c>
     </row>
@@ -4634,103 +4634,103 @@
         <v>14</v>
       </c>
       <c r="B16" s="14">
-        <f>$A16 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>350</v>
       </c>
       <c r="C16" s="8">
-        <f>$A16 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>351</v>
       </c>
       <c r="D16" s="8">
-        <f>$A16 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>352</v>
       </c>
       <c r="E16" s="8">
-        <f>$A16 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>353</v>
       </c>
       <c r="F16" s="8">
-        <f>$A16 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>354</v>
       </c>
       <c r="G16" s="8">
-        <f>$A16 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>355</v>
       </c>
       <c r="H16" s="3">
-        <f>$A16 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>356</v>
       </c>
       <c r="I16" s="3">
-        <f>$A16 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>357</v>
       </c>
       <c r="J16" s="3">
-        <f>$A16 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>358</v>
       </c>
       <c r="K16" s="1">
-        <f>$A16 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>359</v>
       </c>
       <c r="L16" s="1">
-        <f>$A16 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="M16" s="1">
-        <f>$A16 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="N16" s="1">
-        <f>$A16 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>362</v>
       </c>
       <c r="O16" s="1">
-        <f>$A16 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>363</v>
       </c>
       <c r="P16" s="1">
-        <f>$A16 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>364</v>
       </c>
       <c r="Q16" s="1">
-        <f>$A16 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>365</v>
       </c>
       <c r="R16" s="3">
-        <f>$A16 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="S16" s="3">
-        <f>$A16 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>367</v>
       </c>
       <c r="T16" s="3">
-        <f>$A16 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>368</v>
       </c>
       <c r="U16" s="8">
-        <f>$A16 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>369</v>
       </c>
       <c r="V16" s="8">
-        <f>$A16 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>370</v>
       </c>
       <c r="W16" s="8">
-        <f>$A16 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>371</v>
       </c>
       <c r="X16" s="8">
-        <f>$A16 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>372</v>
       </c>
       <c r="Y16" s="8">
-        <f>$A16 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>373</v>
       </c>
       <c r="Z16" s="10">
-        <f>$A16 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>374</v>
       </c>
     </row>
@@ -4739,103 +4739,103 @@
         <v>15</v>
       </c>
       <c r="B17" s="14">
-        <f>$A17 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>375</v>
       </c>
       <c r="C17" s="8">
-        <f>$A17 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>376</v>
       </c>
       <c r="D17" s="8">
-        <f>$A17 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>377</v>
       </c>
       <c r="E17" s="7">
-        <f>$A17 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>378</v>
       </c>
       <c r="F17" s="8">
-        <f>$A17 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>379</v>
       </c>
       <c r="G17" s="8">
-        <f>$A17 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>380</v>
       </c>
       <c r="H17" s="3">
-        <f>$A17 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>381</v>
       </c>
       <c r="I17" s="3">
-        <f>$A17 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>382</v>
       </c>
       <c r="J17" s="3">
-        <f>$A17 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>383</v>
       </c>
       <c r="K17" s="3">
-        <f>$A17 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>384</v>
       </c>
       <c r="L17" s="3">
-        <f>$A17 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>385</v>
       </c>
       <c r="M17" s="3">
-        <f>$A17 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>386</v>
       </c>
       <c r="N17" s="3">
-        <f>$A17 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>387</v>
       </c>
       <c r="O17" s="3">
-        <f>$A17 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>388</v>
       </c>
       <c r="P17" s="3">
-        <f>$A17 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>389</v>
       </c>
       <c r="Q17" s="3">
-        <f>$A17 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>390</v>
       </c>
       <c r="R17" s="3">
-        <f>$A17 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>391</v>
       </c>
       <c r="S17" s="3">
-        <f>$A17 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>392</v>
       </c>
       <c r="T17" s="3">
-        <f>$A17 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>393</v>
       </c>
       <c r="U17" s="8">
-        <f>$A17 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>394</v>
       </c>
       <c r="V17" s="8">
-        <f>$A17 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>395</v>
       </c>
       <c r="W17" s="8">
-        <f>$A17 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>396</v>
       </c>
       <c r="X17" s="8">
-        <f>$A17 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>397</v>
       </c>
       <c r="Y17" s="8">
-        <f>$A17 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>398</v>
       </c>
       <c r="Z17" s="10">
-        <f>$A17 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>399</v>
       </c>
     </row>
@@ -4844,103 +4844,103 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <f>$A18 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="C18" s="3">
-        <f>$A18 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>401</v>
       </c>
       <c r="D18" s="3">
-        <f>$A18 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>402</v>
       </c>
       <c r="E18" s="3">
-        <f>$A18 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>403</v>
       </c>
       <c r="F18" s="3">
-        <f>$A18 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>404</v>
       </c>
       <c r="G18" s="3">
-        <f>$A18 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>405</v>
       </c>
       <c r="H18" s="3">
-        <f>$A18 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>406</v>
       </c>
       <c r="I18" s="35">
-        <f>$A18 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>407</v>
       </c>
       <c r="J18" s="3">
-        <f>$A18 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>408</v>
       </c>
       <c r="K18" s="3">
-        <f>$A18 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>409</v>
       </c>
       <c r="L18" s="3">
-        <f>$A18 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>410</v>
       </c>
       <c r="M18" s="3">
-        <f>$A18 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>411</v>
       </c>
       <c r="N18" s="3">
-        <f>$A18 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>412</v>
       </c>
       <c r="O18" s="3">
-        <f>$A18 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>413</v>
       </c>
       <c r="P18" s="3">
-        <f>$A18 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>414</v>
       </c>
       <c r="Q18" s="3">
-        <f>$A18 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>415</v>
       </c>
       <c r="R18" s="3">
-        <f>$A18 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>416</v>
       </c>
       <c r="S18" s="21">
-        <f>$A18 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>417</v>
       </c>
       <c r="T18" s="3">
-        <f>$A18 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>418</v>
       </c>
       <c r="U18" s="3">
-        <f>$A18 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>419</v>
       </c>
       <c r="V18" s="3">
-        <f>$A18 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>420</v>
       </c>
       <c r="W18" s="3">
-        <f>$A18 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>421</v>
       </c>
       <c r="X18" s="3">
-        <f>$A18 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>422</v>
       </c>
       <c r="Y18" s="3">
-        <f>$A18 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>423</v>
       </c>
       <c r="Z18" s="6">
-        <f>$A18 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>424</v>
       </c>
     </row>
@@ -4949,103 +4949,103 @@
         <v>17</v>
       </c>
       <c r="B19" s="24">
-        <f>$A19 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>425</v>
       </c>
       <c r="C19" s="3">
-        <f>$A19 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>426</v>
       </c>
       <c r="D19" s="3">
-        <f>$A19 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>427</v>
       </c>
       <c r="E19" s="3">
-        <f>$A19 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>428</v>
       </c>
       <c r="F19" s="3">
-        <f>$A19 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>429</v>
       </c>
       <c r="G19" s="3">
-        <f>$A19 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>430</v>
       </c>
       <c r="H19" s="3">
-        <f>$A19 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>431</v>
       </c>
       <c r="I19" s="3">
-        <f>$A19 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>432</v>
       </c>
       <c r="J19" s="3">
-        <f>$A19 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>433</v>
       </c>
       <c r="K19" s="3">
-        <f>$A19 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>434</v>
       </c>
       <c r="L19" s="8">
-        <f>$A19 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>435</v>
       </c>
       <c r="M19" s="7">
-        <f>$A19 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>436</v>
       </c>
       <c r="N19" s="32">
-        <f>$A19 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>437</v>
       </c>
       <c r="O19" s="7">
-        <f>$A19 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>438</v>
       </c>
       <c r="P19" s="8">
-        <f>$A19 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>439</v>
       </c>
       <c r="Q19" s="3">
-        <f>$A19 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>440</v>
       </c>
       <c r="R19" s="3">
-        <f>$A19 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>441</v>
       </c>
       <c r="S19" s="3">
-        <f>$A19 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>442</v>
       </c>
       <c r="T19" s="3">
-        <f>$A19 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>443</v>
       </c>
       <c r="U19" s="3">
-        <f>$A19 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>444</v>
       </c>
       <c r="V19" s="33">
-        <f>$A19 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>445</v>
       </c>
       <c r="W19" s="3">
-        <f>$A19 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>446</v>
       </c>
       <c r="X19" s="3">
-        <f>$A19 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>447</v>
       </c>
       <c r="Y19" s="3">
-        <f>$A19 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>448</v>
       </c>
       <c r="Z19" s="6">
-        <f>$A19 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>449</v>
       </c>
     </row>
@@ -5054,103 +5054,103 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <f>$A20 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="C20" s="8">
-        <f>$A20 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>451</v>
       </c>
       <c r="D20" s="8">
-        <f>$A20 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>452</v>
       </c>
       <c r="E20" s="8">
-        <f>$A20 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>453</v>
       </c>
       <c r="F20" s="8">
-        <f>$A20 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>454</v>
       </c>
       <c r="G20" s="3">
-        <f>$A20 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="H20" s="3">
-        <f>$A20 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>456</v>
       </c>
       <c r="I20" s="3">
-        <f>$A20 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>457</v>
       </c>
       <c r="J20" s="3">
-        <f>$A20 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="K20" s="8">
-        <f>$A20 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="L20" s="8">
-        <f>$A20 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>460</v>
       </c>
       <c r="M20" s="8">
-        <f>$A20 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>461</v>
       </c>
       <c r="N20" s="8">
-        <f>$A20 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>462</v>
       </c>
       <c r="O20" s="8">
-        <f>$A20 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>463</v>
       </c>
       <c r="P20" s="8">
-        <f>$A20 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>464</v>
       </c>
       <c r="Q20" s="8">
-        <f>$A20 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>465</v>
       </c>
       <c r="R20" s="3">
-        <f>$A20 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>466</v>
       </c>
       <c r="S20" s="3">
-        <f>$A20 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>467</v>
       </c>
       <c r="T20" s="36">
-        <f>$A20 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>468</v>
       </c>
       <c r="U20" s="3">
-        <f>$A20 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>469</v>
       </c>
       <c r="V20" s="7">
-        <f>$A20 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>470</v>
       </c>
       <c r="W20" s="8">
-        <f>$A20 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>471</v>
       </c>
       <c r="X20" s="8">
-        <f>$A20 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>472</v>
       </c>
       <c r="Y20" s="8">
-        <f>$A20 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>473</v>
       </c>
       <c r="Z20" s="10">
-        <f>$A20 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>474</v>
       </c>
     </row>
@@ -5159,103 +5159,103 @@
         <v>19</v>
       </c>
       <c r="B21" s="14">
-        <f>$A21 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>475</v>
       </c>
       <c r="C21" s="8">
-        <f>$A21 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>476</v>
       </c>
       <c r="D21" s="8">
-        <f>$A21 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>477</v>
       </c>
       <c r="E21" s="8">
-        <f>$A21 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>478</v>
       </c>
       <c r="F21" s="7">
-        <f>$A21 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>479</v>
       </c>
       <c r="G21" s="3">
-        <f>$A21 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
       <c r="H21" s="3">
-        <f>$A21 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>481</v>
       </c>
       <c r="I21" s="3">
-        <f>$A21 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>482</v>
       </c>
       <c r="J21" s="3">
-        <f>$A21 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>483</v>
       </c>
       <c r="K21" s="8">
-        <f>$A21 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>484</v>
       </c>
       <c r="L21" s="8">
-        <f>$A21 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>485</v>
       </c>
       <c r="M21" s="8">
-        <f>$A21 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>486</v>
       </c>
       <c r="N21" s="8">
-        <f>$A21 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>487</v>
       </c>
       <c r="O21" s="8">
-        <f>$A21 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>488</v>
       </c>
       <c r="P21" s="8">
-        <f>$A21 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>489</v>
       </c>
       <c r="Q21" s="8">
-        <f>$A21 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>490</v>
       </c>
       <c r="R21" s="3">
-        <f>$A21 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>491</v>
       </c>
       <c r="S21" s="3">
-        <f>$A21 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>492</v>
       </c>
       <c r="T21" s="30">
-        <f>$A21 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>493</v>
       </c>
       <c r="U21" s="8">
-        <f>$A21 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>494</v>
       </c>
       <c r="V21" s="8">
-        <f>$A21 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>495</v>
       </c>
       <c r="W21" s="8">
-        <f>$A21 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>496</v>
       </c>
       <c r="X21" s="8">
-        <f>$A21 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>497</v>
       </c>
       <c r="Y21" s="8">
-        <f>$A21 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>498</v>
       </c>
       <c r="Z21" s="10">
-        <f>$A21 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>499</v>
       </c>
     </row>
@@ -5264,103 +5264,103 @@
         <v>20</v>
       </c>
       <c r="B22" s="14">
-        <f>$A22 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="C22" s="8">
-        <f>$A22 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>501</v>
       </c>
       <c r="D22" s="8">
-        <f>$A22 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>502</v>
       </c>
       <c r="E22" s="8">
-        <f>$A22 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>503</v>
       </c>
       <c r="F22" s="37">
-        <f>$A22 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>504</v>
       </c>
       <c r="G22" s="3">
-        <f>$A22 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>505</v>
       </c>
       <c r="H22" s="3">
-        <f>$A22 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>506</v>
       </c>
       <c r="I22" s="3">
-        <f>$A22 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>507</v>
       </c>
       <c r="J22" s="3">
-        <f>$A22 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>508</v>
       </c>
       <c r="K22" s="7">
-        <f>$A22 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>509</v>
       </c>
       <c r="L22" s="8">
-        <f>$A22 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>510</v>
       </c>
       <c r="M22" s="8">
-        <f>$A22 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>511</v>
       </c>
       <c r="N22" s="8">
-        <f>$A22 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="O22" s="8">
-        <f>$A22 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>513</v>
       </c>
       <c r="P22" s="8">
-        <f>$A22 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>514</v>
       </c>
       <c r="Q22" s="8">
-        <f>$A22 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>515</v>
       </c>
       <c r="R22" s="3">
-        <f>$A22 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>516</v>
       </c>
       <c r="S22" s="3">
-        <f>$A22 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>517</v>
       </c>
       <c r="T22" s="7">
-        <f>$A22 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>518</v>
       </c>
       <c r="U22" s="8">
-        <f>$A22 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>519</v>
       </c>
       <c r="V22" s="8">
-        <f>$A22 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>520</v>
       </c>
       <c r="W22" s="8">
-        <f>$A22 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>521</v>
       </c>
       <c r="X22" s="8">
-        <f>$A22 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>522</v>
       </c>
       <c r="Y22" s="8">
-        <f>$A22 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>523</v>
       </c>
       <c r="Z22" s="10">
-        <f>$A22 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>524</v>
       </c>
     </row>
@@ -5369,103 +5369,103 @@
         <v>21</v>
       </c>
       <c r="B23" s="14">
-        <f>$A23 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>525</v>
       </c>
       <c r="C23" s="8">
-        <f>$A23 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>526</v>
       </c>
       <c r="D23" s="8">
-        <f>$A23 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>527</v>
       </c>
       <c r="E23" s="8">
-        <f>$A23 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>528</v>
       </c>
       <c r="F23" s="8">
-        <f>$A23 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>529</v>
       </c>
       <c r="G23" s="3">
-        <f>$A23 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>530</v>
       </c>
       <c r="H23" s="3">
-        <f>$A23 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>531</v>
       </c>
       <c r="I23" s="3">
-        <f>$A23 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>532</v>
       </c>
       <c r="J23" s="3">
-        <f>$A23 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>533</v>
       </c>
       <c r="K23" s="8">
-        <f>$A23 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>534</v>
       </c>
       <c r="L23" s="8">
-        <f>$A23 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>535</v>
       </c>
       <c r="M23" s="8">
-        <f>$A23 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>536</v>
       </c>
       <c r="N23" s="8">
-        <f>$A23 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>537</v>
       </c>
       <c r="O23" s="8">
-        <f>$A23 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>538</v>
       </c>
       <c r="P23" s="8">
-        <f>$A23 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>539</v>
       </c>
       <c r="Q23" s="8">
-        <f>$A23 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>540</v>
       </c>
       <c r="R23" s="3">
-        <f>$A23 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>541</v>
       </c>
       <c r="S23" s="3">
-        <f>$A23 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>542</v>
       </c>
       <c r="T23" s="8">
-        <f>$A23 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>543</v>
       </c>
       <c r="U23" s="8">
-        <f>$A23 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>544</v>
       </c>
       <c r="V23" s="8">
-        <f>$A23 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>545</v>
       </c>
       <c r="W23" s="8">
-        <f>$A23 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>546</v>
       </c>
       <c r="X23" s="8">
-        <f>$A23 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>547</v>
       </c>
       <c r="Y23" s="8">
-        <f>$A23 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>548</v>
       </c>
       <c r="Z23" s="10">
-        <f>$A23 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>549</v>
       </c>
     </row>
@@ -5474,103 +5474,103 @@
         <v>22</v>
       </c>
       <c r="B24" s="14">
-        <f>$A24 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="C24" s="8">
-        <f>$A24 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>551</v>
       </c>
       <c r="D24" s="8">
-        <f>$A24 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>552</v>
       </c>
       <c r="E24" s="8">
-        <f>$A24 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>553</v>
       </c>
       <c r="F24" s="8">
-        <f>$A24 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>554</v>
       </c>
       <c r="G24" s="8">
-        <f>$A24 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>555</v>
       </c>
       <c r="H24" s="3">
-        <f>$A24 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>556</v>
       </c>
       <c r="I24" s="3">
-        <f>$A24 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>557</v>
       </c>
       <c r="J24" s="3">
-        <f>$A24 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>558</v>
       </c>
       <c r="K24" s="8">
-        <f>$A24 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>559</v>
       </c>
       <c r="L24" s="8">
-        <f>$A24 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>560</v>
       </c>
       <c r="M24" s="8">
-        <f>$A24 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>561</v>
       </c>
       <c r="N24" s="8">
-        <f>$A24 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>562</v>
       </c>
       <c r="O24" s="8">
-        <f>$A24 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>563</v>
       </c>
       <c r="P24" s="8">
-        <f>$A24 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>564</v>
       </c>
       <c r="Q24" s="8">
-        <f>$A24 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>565</v>
       </c>
       <c r="R24" s="3">
-        <f>$A24 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>566</v>
       </c>
       <c r="S24" s="28">
-        <f>$A24 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>567</v>
       </c>
       <c r="T24" s="8">
-        <f>$A24 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>568</v>
       </c>
       <c r="U24" s="8">
-        <f>$A24 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>569</v>
       </c>
       <c r="V24" s="8">
-        <f>$A24 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>570</v>
       </c>
       <c r="W24" s="8">
-        <f>$A24 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>571</v>
       </c>
       <c r="X24" s="8">
-        <f>$A24 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>572</v>
       </c>
       <c r="Y24" s="8">
-        <f>$A24 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>573</v>
       </c>
       <c r="Z24" s="10">
-        <f>$A24 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>574</v>
       </c>
     </row>
@@ -5579,103 +5579,103 @@
         <v>23</v>
       </c>
       <c r="B25" s="14">
-        <f>$A25 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>575</v>
       </c>
       <c r="C25" s="8">
-        <f>$A25 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>576</v>
       </c>
       <c r="D25" s="8">
-        <f>$A25 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>577</v>
       </c>
       <c r="E25" s="8">
-        <f>$A25 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>578</v>
       </c>
       <c r="F25" s="8">
-        <f>$A25 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>579</v>
       </c>
       <c r="G25" s="8">
-        <f>$A25 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>580</v>
       </c>
       <c r="H25" s="3">
-        <f>$A25 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>581</v>
       </c>
       <c r="I25" s="3">
-        <f>$A25 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>582</v>
       </c>
       <c r="J25" s="3">
-        <f>$A25 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>583</v>
       </c>
       <c r="K25" s="8">
-        <f>$A25 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>584</v>
       </c>
       <c r="L25" s="8">
-        <f>$A25 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>585</v>
       </c>
       <c r="M25" s="8">
-        <f>$A25 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>586</v>
       </c>
       <c r="N25" s="8">
-        <f>$A25 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>587</v>
       </c>
       <c r="O25" s="8">
-        <f>$A25 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>588</v>
       </c>
       <c r="P25" s="8">
-        <f>$A25 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>589</v>
       </c>
       <c r="Q25" s="8">
-        <f>$A25 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>590</v>
       </c>
       <c r="R25" s="3">
-        <f>$A25 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>591</v>
       </c>
       <c r="S25" s="3">
-        <f>$A25 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>592</v>
       </c>
       <c r="T25" s="8">
-        <f>$A25 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>593</v>
       </c>
       <c r="U25" s="8">
-        <f>$A25 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>594</v>
       </c>
       <c r="V25" s="8">
-        <f>$A25 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>595</v>
       </c>
       <c r="W25" s="8">
-        <f>$A25 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>596</v>
       </c>
       <c r="X25" s="8">
-        <f>$A25 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>597</v>
       </c>
       <c r="Y25" s="8">
-        <f>$A25 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>598</v>
       </c>
       <c r="Z25" s="10">
-        <f>$A25 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>599</v>
       </c>
     </row>
@@ -5684,103 +5684,103 @@
         <v>24</v>
       </c>
       <c r="B26" s="19">
-        <f>$A26 *25 + B$1</f>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="C26" s="9">
-        <f>$A26 *25 + C$1</f>
+        <f t="shared" si="2"/>
         <v>601</v>
       </c>
       <c r="D26" s="9">
-        <f>$A26 *25 + D$1</f>
+        <f t="shared" si="2"/>
         <v>602</v>
       </c>
       <c r="E26" s="9">
-        <f>$A26 *25 + E$1</f>
+        <f t="shared" si="2"/>
         <v>603</v>
       </c>
       <c r="F26" s="9">
-        <f>$A26 *25 + F$1</f>
+        <f t="shared" si="2"/>
         <v>604</v>
       </c>
       <c r="G26" s="9">
-        <f>$A26 *25 + G$1</f>
+        <f t="shared" si="2"/>
         <v>605</v>
       </c>
       <c r="H26" s="4">
-        <f>$A26 *25 + H$1</f>
+        <f t="shared" si="2"/>
         <v>606</v>
       </c>
       <c r="I26" s="23">
-        <f>$A26 *25 + I$1</f>
+        <f t="shared" si="2"/>
         <v>607</v>
       </c>
       <c r="J26" s="4">
-        <f>$A26 *25 + J$1</f>
+        <f t="shared" si="2"/>
         <v>608</v>
       </c>
       <c r="K26" s="4">
-        <f>$A26 *25 + K$1</f>
+        <f t="shared" si="2"/>
         <v>609</v>
       </c>
       <c r="L26" s="9">
-        <f>$A26 *25 + L$1</f>
+        <f t="shared" si="3"/>
         <v>610</v>
       </c>
       <c r="M26" s="9">
-        <f>$A26 *25 + M$1</f>
+        <f t="shared" si="3"/>
         <v>611</v>
       </c>
       <c r="N26" s="9">
-        <f>$A26 *25 + N$1</f>
+        <f t="shared" si="3"/>
         <v>612</v>
       </c>
       <c r="O26" s="9">
-        <f>$A26 *25 + O$1</f>
+        <f t="shared" si="3"/>
         <v>613</v>
       </c>
       <c r="P26" s="9">
-        <f>$A26 *25 + P$1</f>
+        <f t="shared" si="3"/>
         <v>614</v>
       </c>
       <c r="Q26" s="4">
-        <f>$A26 *25 + Q$1</f>
+        <f t="shared" si="3"/>
         <v>615</v>
       </c>
       <c r="R26" s="4">
-        <f>$A26 *25 + R$1</f>
+        <f t="shared" si="3"/>
         <v>616</v>
       </c>
       <c r="S26" s="4">
-        <f>$A26 *25 + S$1</f>
+        <f t="shared" si="3"/>
         <v>617</v>
       </c>
       <c r="T26" s="9">
-        <f>$A26 *25 + T$1</f>
+        <f t="shared" si="3"/>
         <v>618</v>
       </c>
       <c r="U26" s="9">
-        <f>$A26 *25 + U$1</f>
+        <f t="shared" si="3"/>
         <v>619</v>
       </c>
       <c r="V26" s="9">
-        <f>$A26 *25 + V$1</f>
+        <f t="shared" si="3"/>
         <v>620</v>
       </c>
       <c r="W26" s="9">
-        <f>$A26 *25 + W$1</f>
+        <f t="shared" si="3"/>
         <v>621</v>
       </c>
       <c r="X26" s="9">
-        <f>$A26 *25 + X$1</f>
+        <f t="shared" si="3"/>
         <v>622</v>
       </c>
       <c r="Y26" s="9">
-        <f>$A26 *25 + Y$1</f>
+        <f t="shared" si="3"/>
         <v>623</v>
       </c>
       <c r="Z26" s="11">
-        <f>$A26 *25 + Z$1</f>
+        <f t="shared" si="3"/>
         <v>624</v>
       </c>
     </row>

</xml_diff>